<commit_message>
Adding the 3rd party components to BOM with their JLC part numbers.
</commit_message>
<xml_diff>
--- a/Outputs/Assembly/Tangenta-BOM-2024.xlsx
+++ b/Outputs/Assembly/Tangenta-BOM-2024.xlsx
@@ -31,46 +31,7 @@
     <t xml:space="preserve">Footprint</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">JLCPCB Part #</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">（</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">optional</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">）</t>
-    </r>
+    <t xml:space="preserve">JLCPCB Part #</t>
   </si>
   <si>
     <t xml:space="preserve">4.7k</t>
@@ -1137,7 +1098,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="宋体"/>
@@ -1163,13 +1124,6 @@
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="宋体"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -1272,39 +1226,39 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1328,7 +1282,7 @@
   <dimension ref="A1:G137"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D110" activeCellId="0" sqref="D110"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="20.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
New capacitor part number for the TPS buck regulators.
</commit_message>
<xml_diff>
--- a/Outputs/Assembly/Tangenta-BOM-2024.xlsx
+++ b/Outputs/Assembly/Tangenta-BOM-2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="357">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -256,13 +256,16 @@
     <t xml:space="preserve">C220679</t>
   </si>
   <si>
+    <t xml:space="preserve">10uF (47uF EEEFK1V470P)</t>
+  </si>
+  <si>
     <t xml:space="preserve">C3,C2,C5,C4</t>
   </si>
   <si>
     <t xml:space="preserve">CAP_L6</t>
   </si>
   <si>
-    <t xml:space="preserve">C473170</t>
+    <t xml:space="preserve">C178565</t>
   </si>
   <si>
     <t xml:space="preserve">0R</t>
@@ -1282,7 +1285,7 @@
   <dimension ref="A1:G137"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="20.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1671,16 +1674,16 @@
     </row>
     <row r="23" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1688,16 +1691,16 @@
     </row>
     <row r="24" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1705,16 +1708,16 @@
     </row>
     <row r="25" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1722,16 +1725,16 @@
     </row>
     <row r="26" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1739,16 +1742,16 @@
     </row>
     <row r="27" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1759,13 +1762,13 @@
         <v>55</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1773,16 +1776,16 @@
     </row>
     <row r="29" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1790,16 +1793,16 @@
     </row>
     <row r="30" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1807,16 +1810,16 @@
     </row>
     <row r="31" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1824,16 +1827,16 @@
     </row>
     <row r="32" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1841,16 +1844,16 @@
     </row>
     <row r="33" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1861,13 +1864,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1875,16 +1878,16 @@
     </row>
     <row r="35" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>72</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -1892,16 +1895,16 @@
     </row>
     <row r="36" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -1909,16 +1912,16 @@
     </row>
     <row r="37" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1929,13 +1932,13 @@
         <v>100</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -1943,16 +1946,16 @@
     </row>
     <row r="39" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1960,16 +1963,16 @@
     </row>
     <row r="40" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1977,16 +1980,16 @@
     </row>
     <row r="41" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -1994,16 +1997,16 @@
     </row>
     <row r="42" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -2011,16 +2014,16 @@
     </row>
     <row r="43" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -2028,16 +2031,16 @@
     </row>
     <row r="44" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -2045,16 +2048,16 @@
     </row>
     <row r="45" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -2062,16 +2065,16 @@
     </row>
     <row r="46" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -2079,16 +2082,16 @@
     </row>
     <row r="47" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -2096,16 +2099,16 @@
     </row>
     <row r="48" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -2113,16 +2116,16 @@
     </row>
     <row r="49" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -2130,16 +2133,16 @@
     </row>
     <row r="50" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -2147,16 +2150,16 @@
     </row>
     <row r="51" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -2164,16 +2167,16 @@
     </row>
     <row r="52" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -2181,16 +2184,16 @@
     </row>
     <row r="53" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -2198,16 +2201,16 @@
     </row>
     <row r="54" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -2215,16 +2218,16 @@
     </row>
     <row r="55" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -2232,16 +2235,16 @@
     </row>
     <row r="56" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -2249,16 +2252,16 @@
     </row>
     <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -2266,16 +2269,16 @@
     </row>
     <row r="58" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -2283,16 +2286,16 @@
     </row>
     <row r="59" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -2300,16 +2303,16 @@
     </row>
     <row r="60" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -2317,16 +2320,16 @@
     </row>
     <row r="61" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -2334,16 +2337,16 @@
     </row>
     <row r="62" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -2351,16 +2354,16 @@
     </row>
     <row r="63" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -2368,16 +2371,16 @@
     </row>
     <row r="64" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -2385,16 +2388,16 @@
     </row>
     <row r="65" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -2402,16 +2405,16 @@
     </row>
     <row r="66" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -2419,16 +2422,16 @@
     </row>
     <row r="67" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -2436,16 +2439,16 @@
     </row>
     <row r="68" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
@@ -2453,16 +2456,16 @@
     </row>
     <row r="69" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
@@ -2470,16 +2473,16 @@
     </row>
     <row r="70" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -2487,16 +2490,16 @@
     </row>
     <row r="71" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
@@ -2504,16 +2507,16 @@
     </row>
     <row r="72" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -2521,16 +2524,16 @@
     </row>
     <row r="73" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -2538,16 +2541,16 @@
     </row>
     <row r="74" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -2555,16 +2558,16 @@
     </row>
     <row r="75" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
@@ -2572,16 +2575,16 @@
     </row>
     <row r="76" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
@@ -2589,16 +2592,16 @@
     </row>
     <row r="77" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
@@ -2606,16 +2609,16 @@
     </row>
     <row r="78" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
@@ -2623,16 +2626,16 @@
     </row>
     <row r="79" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
@@ -2640,16 +2643,16 @@
     </row>
     <row r="80" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
@@ -2657,16 +2660,16 @@
     </row>
     <row r="81" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
@@ -2674,16 +2677,16 @@
     </row>
     <row r="82" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
@@ -2691,16 +2694,16 @@
     </row>
     <row r="83" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
@@ -2708,16 +2711,16 @@
     </row>
     <row r="84" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
@@ -2725,16 +2728,16 @@
     </row>
     <row r="85" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
@@ -2742,16 +2745,16 @@
     </row>
     <row r="86" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
@@ -2759,16 +2762,16 @@
     </row>
     <row r="87" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
@@ -2776,16 +2779,16 @@
     </row>
     <row r="88" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
@@ -2793,16 +2796,16 @@
     </row>
     <row r="89" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
@@ -2810,16 +2813,16 @@
     </row>
     <row r="90" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
@@ -2827,16 +2830,16 @@
     </row>
     <row r="91" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
@@ -2844,16 +2847,16 @@
     </row>
     <row r="92" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
@@ -2861,16 +2864,16 @@
     </row>
     <row r="93" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
@@ -2878,16 +2881,16 @@
     </row>
     <row r="94" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
@@ -2895,16 +2898,16 @@
     </row>
     <row r="95" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
@@ -2912,16 +2915,16 @@
     </row>
     <row r="96" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
@@ -2929,16 +2932,16 @@
     </row>
     <row r="97" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
@@ -2946,16 +2949,16 @@
     </row>
     <row r="98" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
@@ -2963,16 +2966,16 @@
     </row>
     <row r="99" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
@@ -2980,16 +2983,16 @@
     </row>
     <row r="100" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
@@ -2997,16 +3000,16 @@
     </row>
     <row r="101" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="4" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
@@ -3014,16 +3017,16 @@
     </row>
     <row r="102" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
@@ -3031,16 +3034,16 @@
     </row>
     <row r="103" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
@@ -3048,16 +3051,16 @@
     </row>
     <row r="104" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
@@ -3065,16 +3068,16 @@
     </row>
     <row r="105" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
@@ -3082,16 +3085,16 @@
     </row>
     <row r="106" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
@@ -3099,16 +3102,16 @@
     </row>
     <row r="107" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
@@ -3116,16 +3119,16 @@
     </row>
     <row r="108" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
@@ -3133,16 +3136,16 @@
     </row>
     <row r="109" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="4" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
@@ -3150,16 +3153,16 @@
     </row>
     <row r="110" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C110" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>

</xml_diff>